<commit_message>
SE AGREGA EXTENCION ARCHIVOS CLOUDINARY
</commit_message>
<xml_diff>
--- a/archivos excel/registros_personal_documentacion.xlsx
+++ b/archivos excel/registros_personal_documentacion.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\CAVIJUP\GESTION_HUMANA_CHVS\archivos excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A372AA79-CE6F-4DC3-91A7-52DC33DF6711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2152AD9F-D6C0-4CD2-A277-F800381544FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A0301B53-C6BA-487B-A5DF-9BFDC6363248}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0301B53-C6BA-487B-A5DF-9BFDC6363248}"/>
   </bookViews>
   <sheets>
     <sheet name="RESUMEN DOCUMENTACION ACT" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="credenciales git hub" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'RESUMEN DOCUMENTACION ACT'!$A$2:$CP$19</definedName>
@@ -1527,8 +1527,8 @@
   </sheetPr>
   <dimension ref="A1:CP19"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="O1" zoomScaleNormal="100" zoomScaleSheetLayoutView="10" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CD1" zoomScaleNormal="100" zoomScaleSheetLayoutView="10" workbookViewId="0">
+      <selection activeCell="CI17" sqref="CI17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="BQ4" s="6">
         <f t="shared" ca="1" si="12"/>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="BR4" s="6"/>
       <c r="BS4" s="6"/>
@@ -6231,8 +6231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFAD0BD7-D935-44E5-893C-26B4C33FB087}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: Agregar sistema de envío de correos electrónicos
  - Envío automático de correo de confirmación al usuario
  - Template HTML profesional y responsive
  - Configuración SMTP con Gmail
  - Manejo de errores y logs
  - Notificación al usuario sobre registro recibido
</commit_message>
<xml_diff>
--- a/archivos excel/registros_personal_documentacion.xlsx
+++ b/archivos excel/registros_personal_documentacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\CAVIJUP\GESTION_HUMANA_CHVS\archivos excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2152AD9F-D6C0-4CD2-A277-F800381544FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D1E2E9-7A1A-4CDE-BA6D-8EE98A5ADDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0301B53-C6BA-487B-A5DF-9BFDC6363248}"/>
   </bookViews>
@@ -1527,8 +1527,8 @@
   </sheetPr>
   <dimension ref="A1:CP19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CD1" zoomScaleNormal="100" zoomScaleSheetLayoutView="10" workbookViewId="0">
-      <selection activeCell="CI17" sqref="CI17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="10" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
generaicon de soporte anexo_11
</commit_message>
<xml_diff>
--- a/archivos excel/registros_personal_documentacion.xlsx
+++ b/archivos excel/registros_personal_documentacion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\CAVIJUP\GESTION_HUMANA_CHVS\archivos excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D1E2E9-7A1A-4CDE-BA6D-8EE98A5ADDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6D0D54-21AB-4AE1-8638-6E994FA31110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0301B53-C6BA-487B-A5DF-9BFDC6363248}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1160,7 +1160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1203,13 +1203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1228,9 +1222,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1248,6 +1239,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1527,8 +1524,8 @@
   </sheetPr>
   <dimension ref="A1:CP19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="10" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M2" zoomScaleNormal="100" zoomScaleSheetLayoutView="10" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1585,69 +1582,69 @@
       <c r="A1" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="16" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="18" t="s">
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="18" t="s">
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="R1" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="S1" s="29" t="s">
         <v>269</v>
       </c>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="18" t="s">
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Y1" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="BI1" s="16" t="s">
+      <c r="BI1" s="29" t="s">
         <v>269</v>
       </c>
-      <c r="BJ1" s="16"/>
-      <c r="BK1" s="16"/>
-      <c r="BL1" s="16" t="s">
+      <c r="BJ1" s="29"/>
+      <c r="BK1" s="29"/>
+      <c r="BL1" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="BM1" s="16"/>
-      <c r="BN1" s="16"/>
-      <c r="BO1" s="16"/>
-      <c r="BP1" s="16"/>
-      <c r="BQ1" s="16"/>
-      <c r="BW1" s="18" t="s">
+      <c r="BM1" s="29"/>
+      <c r="BN1" s="29"/>
+      <c r="BO1" s="29"/>
+      <c r="BP1" s="29"/>
+      <c r="BQ1" s="29"/>
+      <c r="BW1" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="BX1" s="18" t="s">
+      <c r="BX1" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="BY1" s="18" t="s">
+      <c r="BY1" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="BZ1" s="18" t="s">
+      <c r="BZ1" s="16" t="s">
         <v>271</v>
       </c>
       <c r="CO1" s="15" t="s">
@@ -1661,283 +1658,283 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="N2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="P2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="26" t="s">
+      <c r="Q2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="27" t="s">
+      <c r="S2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="27" t="s">
+      <c r="T2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="27" t="s">
+      <c r="U2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="26" t="s">
+      <c r="V2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="28" t="s">
+      <c r="W2" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="28" t="s">
+      <c r="X2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="26" t="s">
+      <c r="Y2" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="29" t="s">
+      <c r="Z2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="29" t="s">
+      <c r="AA2" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="29" t="s">
+      <c r="AB2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="29" t="s">
+      <c r="AC2" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="29" t="s">
+      <c r="AD2" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="29" t="s">
+      <c r="AE2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="29" t="s">
+      <c r="AF2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="AG2" s="29" t="s">
+      <c r="AG2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AH2" s="29" t="s">
+      <c r="AH2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="AI2" s="29" t="s">
+      <c r="AI2" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="AJ2" s="29" t="s">
+      <c r="AJ2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="AK2" s="29" t="s">
+      <c r="AK2" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="AL2" s="29" t="s">
+      <c r="AL2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="AM2" s="29" t="s">
+      <c r="AM2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="AN2" s="29" t="s">
+      <c r="AN2" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="AO2" s="29" t="s">
+      <c r="AO2" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="AP2" s="29" t="s">
+      <c r="AP2" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="AQ2" s="29" t="s">
+      <c r="AQ2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="AR2" s="29" t="s">
+      <c r="AR2" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="AS2" s="29" t="s">
+      <c r="AS2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="AT2" s="29" t="s">
+      <c r="AT2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="AU2" s="29" t="s">
+      <c r="AU2" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="AV2" s="29" t="s">
+      <c r="AV2" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="AW2" s="29" t="s">
+      <c r="AW2" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="AX2" s="29" t="s">
+      <c r="AX2" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AY2" s="29" t="s">
+      <c r="AY2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="AZ2" s="29" t="s">
+      <c r="AZ2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="BA2" s="29" t="s">
+      <c r="BA2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="BB2" s="29" t="s">
+      <c r="BB2" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="BC2" s="29" t="s">
+      <c r="BC2" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="BD2" s="29" t="s">
+      <c r="BD2" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="BE2" s="29" t="s">
+      <c r="BE2" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="BF2" s="29" t="s">
+      <c r="BF2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="BG2" s="29" t="s">
+      <c r="BG2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="BH2" s="29" t="s">
+      <c r="BH2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="BI2" s="30" t="s">
+      <c r="BI2" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="BJ2" s="30" t="s">
+      <c r="BJ2" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="BK2" s="30" t="s">
+      <c r="BK2" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="BL2" s="26" t="s">
+      <c r="BL2" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="BM2" s="26" t="s">
+      <c r="BM2" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="BN2" s="26" t="s">
+      <c r="BN2" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="BO2" s="26" t="s">
+      <c r="BO2" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="BP2" s="26" t="s">
+      <c r="BP2" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="BQ2" s="26" t="s">
+      <c r="BQ2" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="BR2" s="29" t="s">
+      <c r="BR2" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="BS2" s="29" t="s">
+      <c r="BS2" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="BT2" s="29" t="s">
+      <c r="BT2" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="BU2" s="29" t="s">
+      <c r="BU2" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="BV2" s="29" t="s">
+      <c r="BV2" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="BW2" s="26" t="s">
+      <c r="BW2" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="BX2" s="26" t="s">
+      <c r="BX2" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="BY2" s="26" t="s">
+      <c r="BY2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BZ2" s="26" t="s">
+      <c r="BZ2" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="CA2" s="29" t="s">
+      <c r="CA2" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="CB2" s="29" t="s">
+      <c r="CB2" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="CC2" s="29" t="s">
+      <c r="CC2" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="CD2" s="29" t="s">
+      <c r="CD2" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="CE2" s="29" t="s">
+      <c r="CE2" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="CF2" s="29" t="s">
+      <c r="CF2" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="CG2" s="29" t="s">
+      <c r="CG2" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="CH2" s="29" t="s">
+      <c r="CH2" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="CI2" s="29" t="s">
+      <c r="CI2" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="CJ2" s="29" t="s">
+      <c r="CJ2" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="CK2" s="29" t="s">
+      <c r="CK2" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="CL2" s="29" t="s">
+      <c r="CL2" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="CM2" s="29" t="s">
+      <c r="CM2" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="CN2" s="19" t="s">
+      <c r="CN2" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="CO2" s="31" t="s">
+      <c r="CO2" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="CP2" s="31" t="s">
+      <c r="CP2" s="28" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4157,7 +4154,7 @@
       </c>
       <c r="BQ11" s="6">
         <f t="shared" ca="1" si="12"/>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="BR11" s="6"/>
       <c r="BS11" s="6"/>

</xml_diff>

<commit_message>
se elimina campo anexo 15
</commit_message>
<xml_diff>
--- a/archivos excel/registros_personal_documentacion.xlsx
+++ b/archivos excel/registros_personal_documentacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\CAVIJUP\GESTION_HUMANA_CHVS\archivos excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6D0D54-21AB-4AE1-8638-6E994FA31110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F59DD04-FC83-4669-B8E0-D5DA88728026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0301B53-C6BA-487B-A5DF-9BFDC6363248}"/>
   </bookViews>
@@ -1524,8 +1524,8 @@
   </sheetPr>
   <dimension ref="A1:CP19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M2" zoomScaleNormal="100" zoomScaleSheetLayoutView="10" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BX1" zoomScaleNormal="100" zoomScaleSheetLayoutView="10" workbookViewId="0">
+      <selection activeCell="CB18" sqref="CB18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
se actualizan campos de las tablas
</commit_message>
<xml_diff>
--- a/archivos excel/registros_personal_documentacion.xlsx
+++ b/archivos excel/registros_personal_documentacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\CAVIJUP\GESTION_HUMANA_CHVS\archivos excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F59DD04-FC83-4669-B8E0-D5DA88728026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5195EA53-98E1-4253-828B-990FD5271B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0301B53-C6BA-487B-A5DF-9BFDC6363248}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A0301B53-C6BA-487B-A5DF-9BFDC6363248}"/>
   </bookViews>
   <sheets>
     <sheet name="RESUMEN DOCUMENTACION ACT" sheetId="1" r:id="rId1"/>
@@ -1524,7 +1524,7 @@
   </sheetPr>
   <dimension ref="A1:CP19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BX1" zoomScaleNormal="100" zoomScaleSheetLayoutView="10" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="CD1" zoomScaleNormal="100" zoomScaleSheetLayoutView="10" workbookViewId="0">
       <selection activeCell="CB18" sqref="CB18"/>
     </sheetView>
   </sheetViews>
@@ -6228,8 +6228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFAD0BD7-D935-44E5-893C-26B4C33FB087}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>